<commit_message>
Se agrega un mínimo de pips para que genere una señal creíble, se configura en config.yaml
</commit_message>
<xml_diff>
--- a/outputs/backtest/summary_best_runs.xlsx
+++ b/outputs/backtest/summary_best_runs.xlsx
@@ -124,7 +124,7 @@
     <t>multiplicative</t>
   </si>
   <si>
-    <t>stacked_lstm</t>
+    <t>bidirectional_lstm</t>
   </si>
 </sst>
 </file>
@@ -588,46 +588,46 @@
         <v>31</v>
       </c>
       <c r="B2">
-        <v>0.003093</v>
+        <v>0.006527</v>
       </c>
       <c r="C2">
-        <v>0.002953</v>
+        <v>0.004222</v>
       </c>
       <c r="D2">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E2">
-        <v>-0.194129</v>
+        <v>-1.535421</v>
       </c>
       <c r="F2">
-        <v>0.846075</v>
+        <v>0.12468</v>
       </c>
       <c r="G2">
-        <v>9.948499999999999</v>
+        <v>9.456235</v>
       </c>
       <c r="H2">
-        <v>150.722054</v>
+        <v>54.887629</v>
       </c>
       <c r="I2">
-        <v>-0.002507</v>
+        <v>-0.003357</v>
       </c>
       <c r="J2">
-        <v>4.727513</v>
+        <v>9.094822000000001</v>
       </c>
       <c r="K2">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="L2">
-        <v>3.151675</v>
+        <v>3.031607</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:31">
@@ -635,52 +635,52 @@
         <v>32</v>
       </c>
       <c r="B3">
-        <v>0.003586</v>
+        <v>0.007225</v>
       </c>
       <c r="C3">
-        <v>0.003121</v>
+        <v>0.004847</v>
       </c>
       <c r="D3">
-        <v>60</v>
+        <v>66.666667</v>
       </c>
       <c r="E3">
-        <v>0.7090689999999999</v>
+        <v>-0.776621</v>
       </c>
       <c r="F3">
-        <v>0.478282</v>
+        <v>0.437383</v>
       </c>
       <c r="G3">
-        <v>1.216381</v>
+        <v>5.143012</v>
       </c>
       <c r="H3">
-        <v>27.244907</v>
+        <v>15.873702</v>
       </c>
       <c r="I3">
-        <v>-0.003978</v>
+        <v>-0.009551</v>
       </c>
       <c r="J3">
-        <v>1.214366</v>
+        <v>2.895164</v>
       </c>
       <c r="K3">
-        <v>60</v>
+        <v>66.666667</v>
       </c>
       <c r="L3">
-        <v>0.809577</v>
+        <v>1.447582</v>
       </c>
       <c r="W3" t="s">
         <v>36</v>
       </c>
       <c r="X3">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="Y3">
         <v>0.2</v>
       </c>
       <c r="Z3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="AA3">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="AB3">
         <v>0.001</v>
@@ -689,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="AD3">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="AE3">
         <v>20</v>
@@ -700,37 +700,37 @@
         <v>33</v>
       </c>
       <c r="B4">
-        <v>0.00416</v>
+        <v>0.008109</v>
       </c>
       <c r="C4">
-        <v>0.003209</v>
+        <v>0.005323</v>
       </c>
       <c r="D4">
-        <v>60</v>
+        <v>66.666667</v>
       </c>
       <c r="E4">
-        <v>0.407355</v>
+        <v>0.6175349999999999</v>
       </c>
       <c r="F4">
-        <v>0.683747</v>
+        <v>0.536882</v>
       </c>
       <c r="G4">
-        <v>9.948499999999999</v>
+        <v>-0.163401</v>
       </c>
       <c r="H4">
-        <v>150.722054</v>
+        <v>-0.126396</v>
       </c>
       <c r="I4">
-        <v>-0.002507</v>
+        <v>-0.024288</v>
       </c>
       <c r="J4">
-        <v>4.727513</v>
+        <v>0.967888</v>
       </c>
       <c r="K4">
-        <v>60</v>
+        <v>66.666667</v>
       </c>
       <c r="L4">
-        <v>3.151675</v>
+        <v>0.483944</v>
       </c>
       <c r="P4">
         <v>0.1</v>
@@ -742,7 +742,7 @@
         <v>35</v>
       </c>
       <c r="S4">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="T4" t="b">
         <v>1</v>
@@ -759,10 +759,10 @@
         <v>34</v>
       </c>
       <c r="B5">
-        <v>0.003257</v>
+        <v>0.007679</v>
       </c>
       <c r="C5">
-        <v>0.002872</v>
+        <v>0.005059</v>
       </c>
       <c r="D5">
         <v>0</v>

</xml_diff>

<commit_message>
Se actualiza el modelo con la version mas reciente
</commit_message>
<xml_diff>
--- a/outputs/backtest/summary_best_runs.xlsx
+++ b/outputs/backtest/summary_best_runs.xlsx
@@ -14,17 +14,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>model</t>
   </si>
   <si>
+    <t>mae</t>
+  </si>
+  <si>
     <t>rmse</t>
   </si>
   <si>
-    <t>mae</t>
-  </si>
-  <si>
     <t>hit_rate</t>
   </si>
   <si>
@@ -52,6 +52,12 @@
     <t>payoff_ratio</t>
   </si>
   <si>
+    <t>n_test_points</t>
+  </si>
+  <si>
+    <t>n_trades</t>
+  </si>
+  <si>
     <t>d</t>
   </si>
   <si>
@@ -61,70 +67,10 @@
     <t>q</t>
   </si>
   <si>
-    <t>changepoint_prior_scale</t>
-  </si>
-  <si>
-    <t>daily_seasonality</t>
-  </si>
-  <si>
-    <t>seasonality_mode</t>
-  </si>
-  <si>
-    <t>seasonality_prior_scale</t>
-  </si>
-  <si>
-    <t>use_lagged_regressors</t>
-  </si>
-  <si>
-    <t>weekly_seasonality</t>
-  </si>
-  <si>
-    <t>yearly_seasonality</t>
-  </si>
-  <si>
-    <t>architecture</t>
-  </si>
-  <si>
-    <t>batch_size</t>
-  </si>
-  <si>
-    <t>dropout</t>
-  </si>
-  <si>
-    <t>early_stopping_patience</t>
-  </si>
-  <si>
-    <t>epochs</t>
-  </si>
-  <si>
-    <t>learning_rate</t>
-  </si>
-  <si>
-    <t>n_layers</t>
-  </si>
-  <si>
-    <t>units</t>
-  </si>
-  <si>
-    <t>window</t>
-  </si>
-  <si>
     <t>ARIMA</t>
   </si>
   <si>
-    <t>LSTM</t>
-  </si>
-  <si>
-    <t>PROPHET</t>
-  </si>
-  <si>
     <t>RandomWalk</t>
-  </si>
-  <si>
-    <t>multiplicative</t>
-  </si>
-  <si>
-    <t>bidirectional_lstm</t>
   </si>
 </sst>
 </file>
@@ -482,13 +428,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE5"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,250 +486,102 @@
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="B2">
+        <v>0.002997</v>
+      </c>
+      <c r="C2">
+        <v>0.003957</v>
+      </c>
+      <c r="D2">
+        <v>82.5</v>
+      </c>
+      <c r="E2">
+        <v>-4.266679</v>
+      </c>
+      <c r="F2">
+        <v>2E-05</v>
+      </c>
+      <c r="G2">
+        <v>8.065003000000001</v>
+      </c>
+      <c r="H2">
+        <v>21.998111</v>
+      </c>
+      <c r="I2">
+        <v>-0.004211</v>
+      </c>
+      <c r="J2">
+        <v>14.190041</v>
+      </c>
+      <c r="K2">
+        <v>82.5</v>
+      </c>
+      <c r="L2">
+        <v>3.010009</v>
+      </c>
+      <c r="M2">
+        <v>160</v>
+      </c>
+      <c r="N2">
+        <v>80</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>2</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2">
-        <v>0.006527</v>
-      </c>
-      <c r="C2">
-        <v>0.004222</v>
-      </c>
-      <c r="D2">
-        <v>75</v>
-      </c>
-      <c r="E2">
-        <v>-1.535421</v>
-      </c>
-      <c r="F2">
-        <v>0.12468</v>
-      </c>
-      <c r="G2">
-        <v>9.456235</v>
-      </c>
-      <c r="H2">
-        <v>54.887629</v>
-      </c>
-      <c r="I2">
-        <v>-0.003357</v>
-      </c>
-      <c r="J2">
-        <v>9.094822000000001</v>
-      </c>
-      <c r="K2">
-        <v>75</v>
-      </c>
-      <c r="L2">
-        <v>3.031607</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>2</v>
-      </c>
-      <c r="O2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
       <c r="B3">
-        <v>0.007225</v>
+        <v>0.005137</v>
       </c>
       <c r="C3">
-        <v>0.004847</v>
+        <v>0.006738</v>
       </c>
       <c r="D3">
-        <v>66.666667</v>
+        <v>52.671756</v>
       </c>
       <c r="E3">
-        <v>-0.776621</v>
+        <v>4.635331</v>
       </c>
       <c r="F3">
-        <v>0.437383</v>
+        <v>4E-06</v>
       </c>
       <c r="G3">
-        <v>5.143012</v>
+        <v>-0.981235</v>
       </c>
       <c r="H3">
-        <v>15.873702</v>
+        <v>-1.265277</v>
       </c>
       <c r="I3">
-        <v>-0.009551</v>
+        <v>-0.06489399999999999</v>
       </c>
       <c r="J3">
-        <v>2.895164</v>
+        <v>0.83242</v>
       </c>
       <c r="K3">
-        <v>66.666667</v>
+        <v>52.671756</v>
       </c>
       <c r="L3">
-        <v>1.447582</v>
-      </c>
-      <c r="W3" t="s">
-        <v>36</v>
-      </c>
-      <c r="X3">
-        <v>32</v>
-      </c>
-      <c r="Y3">
-        <v>0.2</v>
-      </c>
-      <c r="Z3">
-        <v>10</v>
-      </c>
-      <c r="AA3">
-        <v>50</v>
-      </c>
-      <c r="AB3">
-        <v>0.001</v>
-      </c>
-      <c r="AC3">
-        <v>1</v>
-      </c>
-      <c r="AD3">
-        <v>96</v>
-      </c>
-      <c r="AE3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4">
-        <v>0.008109</v>
-      </c>
-      <c r="C4">
-        <v>0.005323</v>
-      </c>
-      <c r="D4">
-        <v>66.666667</v>
-      </c>
-      <c r="E4">
-        <v>0.6175349999999999</v>
-      </c>
-      <c r="F4">
-        <v>0.536882</v>
-      </c>
-      <c r="G4">
-        <v>-0.163401</v>
-      </c>
-      <c r="H4">
-        <v>-0.126396</v>
-      </c>
-      <c r="I4">
-        <v>-0.024288</v>
-      </c>
-      <c r="J4">
-        <v>0.967888</v>
-      </c>
-      <c r="K4">
-        <v>66.666667</v>
-      </c>
-      <c r="L4">
-        <v>0.483944</v>
-      </c>
-      <c r="P4">
-        <v>0.1</v>
-      </c>
-      <c r="Q4" t="b">
-        <v>0</v>
-      </c>
-      <c r="R4" t="s">
-        <v>35</v>
-      </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
-      <c r="T4" t="b">
-        <v>1</v>
-      </c>
-      <c r="U4" t="b">
-        <v>1</v>
-      </c>
-      <c r="V4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5">
-        <v>0.007679</v>
-      </c>
-      <c r="C5">
-        <v>0.005059</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
+        <v>0.747972</v>
+      </c>
+      <c r="M3">
+        <v>160</v>
+      </c>
+      <c r="N3">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>